<commit_message>
minor correction: several excel sheet is not imported
</commit_message>
<xml_diff>
--- a/Data Extraction.xlsx
+++ b/Data Extraction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="958" activeTab="5"/>
+    <workbookView xWindow="29360" yWindow="1160" windowWidth="25600" windowHeight="15480" tabRatio="958" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Mappings" sheetId="12" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="422">
   <si>
     <t>Experiment ID</t>
   </si>
@@ -1123,24 +1123,6 @@
     <t>experimentBok</t>
   </si>
   <si>
-    <t>experimentBokProcess</t>
-  </si>
-  <si>
-    <t>experimentBokActivity</t>
-  </si>
-  <si>
-    <t>experimentBokArtifact</t>
-  </si>
-  <si>
-    <t>experimentBokTechnique</t>
-  </si>
-  <si>
-    <t>experimentBokModel</t>
-  </si>
-  <si>
-    <t>experimentBokTool</t>
-  </si>
-  <si>
     <t>experimentArtifact</t>
   </si>
   <si>
@@ -1388,6 +1370,39 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>Findings</t>
+  </si>
+  <si>
+    <t>Threat to Validity</t>
+  </si>
+  <si>
+    <t>additionalProperty</t>
+  </si>
+  <si>
+    <t>bokTopicType=Process;</t>
+  </si>
+  <si>
+    <t>bokTopicType=Activity;</t>
+  </si>
+  <si>
+    <t>bokTopicType=Artifact;</t>
+  </si>
+  <si>
+    <t>bokTopicType=Defect Detection Technique;</t>
+  </si>
+  <si>
+    <t>bokTopicType=Tool;</t>
+  </si>
+  <si>
+    <t>bokTopicType=Model;</t>
+  </si>
+  <si>
+    <t>hasExperimentBokTopic</t>
+  </si>
+  <si>
+    <t>BokTopic</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1476,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1535,7 +1566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1558,6 +1589,14 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1580,6 +1619,14 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1885,7 +1932,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1978,7 +2025,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2703,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2720,9 +2767,10 @@
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="13" t="s">
         <v>303</v>
       </c>
@@ -2745,401 +2793,443 @@
         <v>309</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1">
-      <c r="A2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="10" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>410</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>410</v>
+      </c>
+      <c r="J4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>410</v>
+      </c>
+      <c r="J5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1">
+      <c r="A6" t="s">
         <v>310</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>410</v>
+      </c>
+      <c r="J6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>410</v>
+      </c>
+      <c r="J7" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>410</v>
+      </c>
+      <c r="J8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>410</v>
+      </c>
+      <c r="J9" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>410</v>
+      </c>
+      <c r="J10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>312</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J11" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B12" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>410</v>
+      </c>
+      <c r="J12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>410</v>
+      </c>
+      <c r="J13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G14" s="10">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E3" t="s">
-        <v>316</v>
-      </c>
-      <c r="F3" t="s">
-        <v>310</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>410</v>
+      </c>
+      <c r="J14" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B15" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>339</v>
-      </c>
-      <c r="E4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E5" t="s">
-        <v>316</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="10" customFormat="1">
-      <c r="A6" t="s">
-        <v>318</v>
-      </c>
-      <c r="B6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>344</v>
-      </c>
-      <c r="E6" t="s">
-        <v>316</v>
-      </c>
-      <c r="F6" t="s">
-        <v>310</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>355</v>
-      </c>
-      <c r="E7" t="s">
-        <v>316</v>
-      </c>
-      <c r="F7" t="s">
-        <v>343</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>300</v>
-      </c>
-      <c r="B8" t="s">
-        <v>300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E8" t="s">
-        <v>316</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="11">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>361</v>
-      </c>
-      <c r="E9" t="s">
-        <v>316</v>
-      </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-      <c r="G9" s="11">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>362</v>
-      </c>
-      <c r="E10" t="s">
-        <v>316</v>
-      </c>
-      <c r="F10" t="s">
-        <v>321</v>
-      </c>
-      <c r="G10" s="11">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>363</v>
-      </c>
-      <c r="E11" t="s">
-        <v>316</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B12" t="s">
-        <v>319</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>379</v>
-      </c>
-      <c r="E12" t="s">
-        <v>316</v>
-      </c>
-      <c r="F12" t="s">
-        <v>343</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B13" t="s">
-        <v>319</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>380</v>
-      </c>
-      <c r="E13" t="s">
-        <v>316</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>320</v>
-      </c>
-      <c r="B14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>386</v>
-      </c>
-      <c r="E14" t="s">
-        <v>316</v>
-      </c>
-      <c r="F14" t="s">
-        <v>310</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>391</v>
+        <v>333</v>
       </c>
       <c r="E15" t="s">
         <v>316</v>
@@ -3147,63 +3237,69 @@
       <c r="F15" t="s">
         <v>310</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="11">
         <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>410</v>
+      </c>
+      <c r="J15" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>365</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G16" s="11">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J16" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" t="s">
-        <v>395</v>
-      </c>
-      <c r="E16" t="s">
-        <v>316</v>
-      </c>
-      <c r="F16" t="s">
-        <v>320</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>323</v>
-      </c>
       <c r="C17" s="10" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>322</v>
+        <v>388</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>314</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G17" s="10">
         <v>0</v>
@@ -3212,114 +3308,126 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="10" customFormat="1">
-      <c r="A18" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10">
+        <v>410</v>
+      </c>
+      <c r="J17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="10" customFormat="1">
+      <c r="A18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" t="s">
+        <v>389</v>
+      </c>
+      <c r="E18" t="s">
+        <v>316</v>
+      </c>
+      <c r="F18" t="s">
+        <v>320</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="J18" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>390</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>411</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J20" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="B21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G19" s="10">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="D21" s="10" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>314</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G21" s="10">
         <v>0</v>
@@ -3328,143 +3436,158 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G22" s="10">
+        <v>410</v>
+      </c>
+      <c r="J21" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="10">
+      <c r="D22" t="s">
+        <v>315</v>
+      </c>
+      <c r="E22" t="s">
+        <v>316</v>
+      </c>
+      <c r="F22" t="s">
+        <v>310</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="10" customFormat="1">
-      <c r="A23" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G23" s="10">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
+        <v>410</v>
+      </c>
+      <c r="J22" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="10" customFormat="1">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G23" s="11">
+        <v>2</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G24" s="10">
-        <v>0</v>
-      </c>
-      <c r="H24" s="10">
+        <v>410</v>
+      </c>
+      <c r="J23" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" t="s">
+        <v>330</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G24" s="11">
+        <v>3</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G25" s="10">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10">
+        <v>410</v>
+      </c>
+      <c r="J24" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" t="s">
+        <v>331</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G25" s="11">
+        <v>4</v>
+      </c>
+      <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="10" customFormat="1">
+        <v>403</v>
+      </c>
+      <c r="J25" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="10" customFormat="1">
       <c r="A26" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>378</v>
+        <v>322</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>314</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G26" s="10">
         <v>0</v>
@@ -3473,552 +3596,609 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="J26" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>317</v>
+      </c>
+      <c r="B27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" t="s">
+        <v>316</v>
+      </c>
+      <c r="F27" t="s">
+        <v>310</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>410</v>
+      </c>
+      <c r="J27" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>317</v>
+      </c>
+      <c r="B28" t="s">
+        <v>323</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>324</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>410</v>
+      </c>
+      <c r="J28" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="10" customFormat="1">
+      <c r="A29" t="s">
+        <v>317</v>
+      </c>
+      <c r="B29" t="s">
+        <v>323</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>325</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>410</v>
+      </c>
+      <c r="J29" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>410</v>
+      </c>
+      <c r="J30" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>355</v>
+      </c>
+      <c r="E31" t="s">
+        <v>316</v>
+      </c>
+      <c r="F31" t="s">
+        <v>300</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>410</v>
+      </c>
+      <c r="J31" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>356</v>
+      </c>
+      <c r="E32" t="s">
+        <v>316</v>
+      </c>
+      <c r="F32" t="s">
+        <v>321</v>
+      </c>
+      <c r="G32" s="11">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>410</v>
+      </c>
+      <c r="J32" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>368</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G33" s="11">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J33" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>357</v>
+      </c>
+      <c r="E34" t="s">
+        <v>316</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="11">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>410</v>
+      </c>
+      <c r="J34" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
+        <v>358</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G35" s="11">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>404</v>
+      </c>
+      <c r="J35" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>359</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G36" s="11">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J36" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>410</v>
+      </c>
+      <c r="J37" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>363</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J38" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>361</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G39" s="11">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>405</v>
+      </c>
+      <c r="J39" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>362</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G40" s="11">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J40" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
+        <v>369</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G41" s="11">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J41" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>370</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G42" s="11">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J42" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="10" customFormat="1">
+      <c r="A43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" t="s">
+        <v>371</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G43" s="11">
+        <v>6</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J43" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="E27" s="10" t="s">
+      <c r="D44" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G27" s="10">
+      <c r="F44" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G44" s="10">
         <v>0</v>
       </c>
-      <c r="H27" s="10">
-        <v>1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G28" s="10">
+      <c r="H44" s="10">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>410</v>
+      </c>
+      <c r="J44" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>320</v>
+      </c>
+      <c r="B45" t="s">
+        <v>320</v>
+      </c>
+      <c r="C45" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="10">
-        <v>1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="10" customFormat="1">
-      <c r="A29" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G29" s="10">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10">
-        <v>1</v>
-      </c>
-      <c r="I29" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
-        <v>317</v>
-      </c>
-      <c r="B30" t="s">
-        <v>323</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" t="s">
-        <v>324</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>317</v>
-      </c>
-      <c r="B31" t="s">
-        <v>323</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" t="s">
-        <v>325</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G31">
-        <v>3</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="D45" t="s">
+        <v>380</v>
+      </c>
+      <c r="E45" t="s">
+        <v>316</v>
+      </c>
+      <c r="F45" t="s">
         <v>310</v>
       </c>
-      <c r="B32" t="s">
-        <v>310</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D32" t="s">
-        <v>326</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>310</v>
-      </c>
-      <c r="B33" t="s">
-        <v>310</v>
-      </c>
-      <c r="C33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" t="s">
-        <v>327</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>310</v>
-      </c>
-      <c r="B34" t="s">
-        <v>310</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" t="s">
-        <v>328</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>310</v>
-      </c>
-      <c r="B35" t="s">
-        <v>310</v>
-      </c>
-      <c r="C35" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" t="s">
-        <v>329</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G35">
-        <v>4</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>310</v>
-      </c>
-      <c r="B36" t="s">
-        <v>310</v>
-      </c>
-      <c r="C36" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" t="s">
-        <v>330</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G36">
-        <v>5</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>310</v>
-      </c>
-      <c r="B37" t="s">
-        <v>310</v>
-      </c>
-      <c r="C37" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" t="s">
-        <v>331</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G37">
-        <v>6</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>310</v>
-      </c>
-      <c r="B38" t="s">
-        <v>310</v>
-      </c>
-      <c r="C38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" t="s">
-        <v>332</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G38">
-        <v>7</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
-        <v>310</v>
-      </c>
-      <c r="B39" t="s">
-        <v>310</v>
-      </c>
-      <c r="C39" t="s">
-        <v>144</v>
-      </c>
-      <c r="D39" t="s">
-        <v>333</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G39">
-        <v>8</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>310</v>
-      </c>
-      <c r="B40" t="s">
-        <v>310</v>
-      </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>312</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G40">
-        <v>9</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>310</v>
-      </c>
-      <c r="B41" t="s">
-        <v>310</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>311</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G41">
-        <v>10</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>310</v>
-      </c>
-      <c r="B42" t="s">
-        <v>310</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" t="s">
-        <v>334</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G42">
-        <v>11</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="I42" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="10" customFormat="1">
-      <c r="A43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>370</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G43" s="11">
-        <v>2</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>130</v>
-      </c>
-      <c r="D44" t="s">
-        <v>336</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G44" s="11">
-        <v>3</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="I44" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" t="s">
-        <v>364</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G45" s="11">
-        <v>5</v>
+      <c r="G45">
+        <v>1</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -4026,25 +4206,28 @@
       <c r="I45" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="C46" t="s">
-        <v>290</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -4052,156 +4235,174 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="I46" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J46" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B47" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>62</v>
       </c>
       <c r="D47" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G47" s="11">
-        <v>8</v>
+        <v>408</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J47" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
-        <v>318</v>
-      </c>
-      <c r="B48" t="s">
-        <v>343</v>
-      </c>
-      <c r="C48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" t="s">
-        <v>348</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G48" s="11">
-        <v>4</v>
-      </c>
-      <c r="H48">
+      <c r="G48" s="10">
+        <v>0</v>
+      </c>
+      <c r="H48" s="10">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>49</v>
+        <v>410</v>
+      </c>
+      <c r="J48" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>321</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>367</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>414</v>
+        <v>336</v>
+      </c>
+      <c r="E49" t="s">
+        <v>316</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
       </c>
       <c r="G49" s="11">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>410</v>
+      </c>
+      <c r="J49" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="10" customFormat="1">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>321</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>366</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G50" s="11">
         <v>2</v>
       </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="10" customFormat="1">
-      <c r="A50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>226</v>
-      </c>
-      <c r="D50" t="s">
-        <v>337</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G50" s="11">
-        <v>4</v>
-      </c>
       <c r="H50">
         <v>1</v>
       </c>
-      <c r="I50" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" t="s">
-        <v>318</v>
-      </c>
-      <c r="B51" t="s">
-        <v>343</v>
-      </c>
-      <c r="C51" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" t="s">
-        <v>401</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G51" s="11">
-        <v>5</v>
-      </c>
-      <c r="H51">
+      <c r="I50" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J50" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G51" s="10">
+        <v>0</v>
+      </c>
+      <c r="H51" s="10">
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>410</v>
+      </c>
+      <c r="J51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>319</v>
       </c>
@@ -4209,930 +4410,1026 @@
         <v>319</v>
       </c>
       <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>373</v>
+      </c>
+      <c r="E52" t="s">
+        <v>316</v>
+      </c>
+      <c r="F52" t="s">
+        <v>337</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>410</v>
+      </c>
+      <c r="J52" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>319</v>
+      </c>
+      <c r="B53" t="s">
+        <v>319</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>374</v>
+      </c>
+      <c r="E53" t="s">
+        <v>316</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>410</v>
+      </c>
+      <c r="J53" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>319</v>
+      </c>
+      <c r="B54" t="s">
+        <v>319</v>
+      </c>
+      <c r="C54" t="s">
         <v>261</v>
       </c>
-      <c r="D52" t="s">
-        <v>381</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G52">
+      <c r="D54" t="s">
+        <v>375</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G54">
         <v>3</v>
       </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" t="s">
+        <v>406</v>
+      </c>
+      <c r="J54" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>319</v>
+      </c>
+      <c r="B55" t="s">
+        <v>319</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>376</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J55" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>319</v>
+      </c>
+      <c r="B56" t="s">
+        <v>319</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" t="s">
+        <v>377</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J56" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="10" customFormat="1">
+      <c r="A57" t="s">
+        <v>319</v>
+      </c>
+      <c r="B57" t="s">
+        <v>319</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>378</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G57">
+        <v>6</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J57" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="B53" t="s">
-        <v>343</v>
-      </c>
-      <c r="C53" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53" t="s">
-        <v>398</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G53" s="11">
+      <c r="B58" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="s">
-        <v>318</v>
-      </c>
-      <c r="B54" t="s">
-        <v>343</v>
-      </c>
-      <c r="C54" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" t="s">
-        <v>399</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G54" s="11">
-        <v>7</v>
-      </c>
-      <c r="H54">
-        <v>1</v>
-      </c>
-      <c r="I54" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>371</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G55" s="11">
-        <v>2</v>
-      </c>
-      <c r="H55">
-        <v>1</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>321</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
-        <v>372</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G56" s="11">
-        <v>2</v>
-      </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="10" customFormat="1">
-      <c r="A57" t="s">
-        <v>318</v>
-      </c>
-      <c r="B57" t="s">
-        <v>343</v>
-      </c>
-      <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" t="s">
-        <v>346</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G57" s="11">
-        <v>2</v>
-      </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="s">
-        <v>318</v>
-      </c>
-      <c r="B58" t="s">
-        <v>343</v>
-      </c>
-      <c r="C58" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" t="s">
-        <v>347</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G58" s="11">
-        <v>3</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="D58" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G58" s="10">
+        <v>0</v>
+      </c>
+      <c r="H58" s="10">
+        <v>1</v>
+      </c>
+      <c r="I58" t="s">
+        <v>410</v>
+      </c>
+      <c r="J58" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>318</v>
       </c>
       <c r="B59" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>349</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>414</v>
+        <v>338</v>
+      </c>
+      <c r="E59" t="s">
+        <v>316</v>
+      </c>
+      <c r="F59" t="s">
+        <v>310</v>
       </c>
       <c r="G59" s="11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
-      <c r="I59" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="I59" t="s">
+        <v>410</v>
+      </c>
+      <c r="J59" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>318</v>
       </c>
       <c r="B60" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G60" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>410</v>
+      </c>
+      <c r="J60" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>318</v>
       </c>
       <c r="B61" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D61" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G61" s="11">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>410</v>
+      </c>
+      <c r="J61" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>318</v>
       </c>
       <c r="B62" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G62" s="11">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
-      <c r="I62" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="I62" t="s">
+        <v>397</v>
+      </c>
+      <c r="J62" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>318</v>
       </c>
       <c r="B63" t="s">
+        <v>337</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" t="s">
+        <v>395</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G63" s="11">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63" t="s">
+        <v>399</v>
+      </c>
+      <c r="J63" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="10" customFormat="1">
+      <c r="A64" t="s">
+        <v>318</v>
+      </c>
+      <c r="B64" t="s">
+        <v>337</v>
+      </c>
+      <c r="C64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" t="s">
+        <v>392</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G64" s="11">
+        <v>6</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>400</v>
+      </c>
+      <c r="J64" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
+        <v>318</v>
+      </c>
+      <c r="B65" t="s">
+        <v>337</v>
+      </c>
+      <c r="C65" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" t="s">
+        <v>393</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G65" s="11">
+        <v>7</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>401</v>
+      </c>
+      <c r="J65" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" t="s">
+        <v>337</v>
+      </c>
+      <c r="C66" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" t="s">
+        <v>394</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G66" s="11">
+        <v>8</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66" t="s">
+        <v>402</v>
+      </c>
+      <c r="J66" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>318</v>
+      </c>
+      <c r="B67" t="s">
+        <v>337</v>
+      </c>
+      <c r="C67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" t="s">
         <v>343</v>
       </c>
-      <c r="C63" t="s">
+      <c r="E67" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G67" s="11">
+        <v>9</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J67" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" t="s">
+        <v>318</v>
+      </c>
+      <c r="B68" t="s">
+        <v>337</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>344</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G68" s="11">
+        <v>10</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J68" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
+        <v>318</v>
+      </c>
+      <c r="B69" t="s">
+        <v>337</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" t="s">
+        <v>345</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G69" s="11">
+        <v>11</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J69" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>318</v>
+      </c>
+      <c r="B70" t="s">
+        <v>337</v>
+      </c>
+      <c r="C70" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" t="s">
+        <v>346</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G70" s="11">
+        <v>12</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J70" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="10" customFormat="1">
+      <c r="A71" t="s">
+        <v>318</v>
+      </c>
+      <c r="B71" t="s">
+        <v>337</v>
+      </c>
+      <c r="C71" t="s">
         <v>67</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D71" t="s">
+        <v>347</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G71" s="11">
+        <v>13</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J71" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G72" s="10">
+        <v>0</v>
+      </c>
+      <c r="H72" s="10">
+        <v>1</v>
+      </c>
+      <c r="I72" t="s">
+        <v>410</v>
+      </c>
+      <c r="J72" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" t="s">
+        <v>412</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>385</v>
+      </c>
+      <c r="E73" t="s">
+        <v>316</v>
+      </c>
+      <c r="F73" t="s">
+        <v>310</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73" t="s">
+        <v>410</v>
+      </c>
+      <c r="J73" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" t="s">
+        <v>412</v>
+      </c>
+      <c r="B74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" t="s">
+        <v>290</v>
+      </c>
+      <c r="D74" t="s">
+        <v>383</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>407</v>
+      </c>
+      <c r="J74" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="10" customFormat="1">
+      <c r="A75" t="s">
+        <v>412</v>
+      </c>
+      <c r="B75" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>386</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J75" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
+        <v>412</v>
+      </c>
+      <c r="B76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C76" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" t="s">
+        <v>387</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G76">
+        <v>4</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J76" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G77" s="10">
+        <v>0</v>
+      </c>
+      <c r="H77" s="10">
+        <v>1</v>
+      </c>
+      <c r="I77" t="s">
+        <v>410</v>
+      </c>
+      <c r="J77" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" t="s">
+        <v>300</v>
+      </c>
+      <c r="B78" t="s">
+        <v>300</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>349</v>
+      </c>
+      <c r="E78" t="s">
+        <v>316</v>
+      </c>
+      <c r="F78" t="s">
+        <v>337</v>
+      </c>
+      <c r="G78" s="11">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>410</v>
+      </c>
+      <c r="J78" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>300</v>
+      </c>
+      <c r="B79" t="s">
+        <v>300</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>350</v>
+      </c>
+      <c r="E79" t="s">
+        <v>316</v>
+      </c>
+      <c r="F79" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="11">
+        <v>2</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>410</v>
+      </c>
+      <c r="J79" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="10" customFormat="1">
+      <c r="A80" t="s">
+        <v>300</v>
+      </c>
+      <c r="B80" t="s">
+        <v>300</v>
+      </c>
+      <c r="C80" t="s">
+        <v>75</v>
+      </c>
+      <c r="D80" t="s">
+        <v>367</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G80" s="11">
+        <v>3</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J80" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" t="s">
+        <v>300</v>
+      </c>
+      <c r="B81" t="s">
+        <v>300</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>351</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G81" s="11">
+        <v>4</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J81" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" t="s">
+        <v>300</v>
+      </c>
+      <c r="B82" t="s">
+        <v>300</v>
+      </c>
+      <c r="C82" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82" t="s">
+        <v>352</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G82" s="11">
+        <v>5</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="J82" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83" t="s">
+        <v>300</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
         <v>353</v>
       </c>
-      <c r="E63" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G63" s="11">
-        <v>13</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
-      </c>
-      <c r="I63" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="10" customFormat="1">
-      <c r="A64" t="s">
-        <v>300</v>
-      </c>
-      <c r="B64" t="s">
-        <v>300</v>
-      </c>
-      <c r="C64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D64" t="s">
-        <v>373</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G64" s="11">
-        <v>3</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" t="s">
-        <v>300</v>
-      </c>
-      <c r="B65" t="s">
-        <v>300</v>
-      </c>
-      <c r="C65" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" t="s">
-        <v>357</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F65" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G65" s="11">
-        <v>4</v>
-      </c>
-      <c r="H65">
-        <v>1</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" t="s">
-        <v>300</v>
-      </c>
-      <c r="B66" t="s">
-        <v>300</v>
-      </c>
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s">
-        <v>358</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G66" s="11">
-        <v>5</v>
-      </c>
-      <c r="H66">
-        <v>1</v>
-      </c>
-      <c r="I66" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" t="s">
-        <v>300</v>
-      </c>
-      <c r="B67" t="s">
-        <v>300</v>
-      </c>
-      <c r="C67" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" t="s">
-        <v>359</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F67" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G67" s="11">
+      <c r="E83" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G83" s="11">
         <v>6</v>
       </c>
-      <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
-        <v>374</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G68" s="11">
-        <v>3</v>
-      </c>
-      <c r="H68">
-        <v>1</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" t="s">
-        <v>365</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G69" s="11">
-        <v>6</v>
-      </c>
-      <c r="H69">
-        <v>1</v>
-      </c>
-      <c r="I69" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" t="s">
-        <v>369</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G70" s="11">
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="10" customFormat="1">
-      <c r="A71" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>368</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G71" s="11">
-        <v>3</v>
-      </c>
-      <c r="H71">
-        <v>1</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D72" t="s">
-        <v>375</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G72" s="11">
-        <v>4</v>
-      </c>
-      <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D73" t="s">
-        <v>376</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G73" s="11">
-        <v>5</v>
-      </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D74" t="s">
-        <v>377</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G74" s="11">
-        <v>6</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="10" customFormat="1">
-      <c r="A75" t="s">
-        <v>319</v>
-      </c>
-      <c r="B75" t="s">
-        <v>319</v>
-      </c>
-      <c r="C75" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" t="s">
-        <v>382</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G75">
-        <v>4</v>
-      </c>
-      <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" t="s">
-        <v>319</v>
-      </c>
-      <c r="B76" t="s">
-        <v>319</v>
-      </c>
-      <c r="C76" t="s">
-        <v>43</v>
-      </c>
-      <c r="D76" t="s">
-        <v>383</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G76">
-        <v>5</v>
-      </c>
-      <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" t="s">
-        <v>319</v>
-      </c>
-      <c r="B77" t="s">
-        <v>319</v>
-      </c>
-      <c r="C77" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G77">
-        <v>6</v>
-      </c>
-      <c r="H77">
-        <v>1</v>
-      </c>
-      <c r="I77" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" t="s">
-        <v>320</v>
-      </c>
-      <c r="B78" t="s">
-        <v>320</v>
-      </c>
-      <c r="C78" t="s">
-        <v>132</v>
-      </c>
-      <c r="D78" t="s">
-        <v>387</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" t="s">
-        <v>320</v>
-      </c>
-      <c r="B79" t="s">
-        <v>320</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79" t="s">
-        <v>388</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F79" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G79">
-        <v>3</v>
-      </c>
-      <c r="H79">
-        <v>1</v>
-      </c>
-      <c r="I79" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" s="10" customFormat="1">
-      <c r="A80" t="s">
-        <v>42</v>
-      </c>
-      <c r="B80" t="s">
-        <v>42</v>
-      </c>
-      <c r="C80" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" t="s">
-        <v>392</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F80" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G80">
-        <v>3</v>
-      </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81" t="s">
-        <v>42</v>
-      </c>
-      <c r="C81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D81" t="s">
-        <v>393</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F81" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G81">
-        <v>4</v>
-      </c>
-      <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="I81" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" t="s">
-        <v>125</v>
-      </c>
-      <c r="C82" t="s">
-        <v>125</v>
-      </c>
-      <c r="D82" t="s">
-        <v>396</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G82">
-        <v>2</v>
-      </c>
-      <c r="H82">
-        <v>1</v>
-      </c>
-      <c r="I82" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" t="s">
-        <v>125</v>
-      </c>
-      <c r="B83" t="s">
-        <v>125</v>
-      </c>
-      <c r="C83" t="s">
-        <v>131</v>
-      </c>
-      <c r="D83" t="s">
-        <v>397</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="G83">
-        <v>3</v>
-      </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>416</v>
+        <v>410</v>
+      </c>
+      <c r="J83" t="s">
+        <v>409</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1">
     <sortState ref="A2:I83">
-      <sortCondition ref="I1:I83"/>
+      <sortCondition ref="B1:B83"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5881,7 +6178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
additional data import configuration - allows creation of class from properties (BoK Topic)
</commit_message>
<xml_diff>
--- a/Data Extraction.xlsx
+++ b/Data Extraction.xlsx
@@ -4,37 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29360" yWindow="1160" windowWidth="25600" windowHeight="15480" tabRatio="958" activeTab="13"/>
+    <workbookView xWindow="27340" yWindow="1080" windowWidth="33600" windowHeight="21000" tabRatio="958"/>
   </bookViews>
   <sheets>
-    <sheet name="Mappings" sheetId="12" r:id="rId1"/>
-    <sheet name="Experiment" sheetId="2" r:id="rId2"/>
-    <sheet name="Hypothesis" sheetId="3" r:id="rId3"/>
-    <sheet name="Factor" sheetId="4" r:id="rId4"/>
-    <sheet name="Response Variable" sheetId="5" r:id="rId5"/>
-    <sheet name="Experiment Run" sheetId="6" r:id="rId6"/>
-    <sheet name="Treatment" sheetId="7" r:id="rId7"/>
-    <sheet name="Measurement" sheetId="8" r:id="rId8"/>
-    <sheet name="Metric" sheetId="11" r:id="rId9"/>
-    <sheet name="Result" sheetId="9" r:id="rId10"/>
-    <sheet name="Publication" sheetId="1" r:id="rId11"/>
-    <sheet name="Threat to Validity" sheetId="10" r:id="rId12"/>
-    <sheet name="Findings" sheetId="13" r:id="rId13"/>
-    <sheet name="Ontology Mapping" sheetId="14" r:id="rId14"/>
+    <sheet name="Concepts" sheetId="16" r:id="rId1"/>
+    <sheet name="Mappings" sheetId="12" r:id="rId2"/>
+    <sheet name="Experiment" sheetId="2" r:id="rId3"/>
+    <sheet name="Hypothesis" sheetId="3" r:id="rId4"/>
+    <sheet name="Factor" sheetId="4" r:id="rId5"/>
+    <sheet name="Response Variable" sheetId="5" r:id="rId6"/>
+    <sheet name="Experiment Run" sheetId="6" r:id="rId7"/>
+    <sheet name="Treatment" sheetId="7" r:id="rId8"/>
+    <sheet name="Measurement" sheetId="8" r:id="rId9"/>
+    <sheet name="Metric" sheetId="11" r:id="rId10"/>
+    <sheet name="Result" sheetId="9" r:id="rId11"/>
+    <sheet name="Publication" sheetId="1" r:id="rId12"/>
+    <sheet name="Threat to Validity" sheetId="10" r:id="rId13"/>
+    <sheet name="Findings" sheetId="13" r:id="rId14"/>
+    <sheet name="Ontology Mapping" sheetId="14" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Experiment!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Experiment Run'!$B$1:$N$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Factor!$A$1:$C$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Findings!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hypothesis!$A$1:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7">Measurement!$B$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Metric!$B$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Ontology Mapping'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Publication!$B$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Response Variable'!$B$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Threat to Validity'!$A$1:$E$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Treatment!$B$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Experiment!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Experiment Run'!$B$1:$N$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Factor!$A$1:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Findings!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hypothesis!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8">Measurement!$B$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Metric!$B$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Ontology Mapping'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Publication!$B$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Response Variable'!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Threat to Validity'!$A$1:$E$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Treatment!$B$1:$G$3</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="436">
   <si>
     <t>Experiment ID</t>
   </si>
@@ -1403,6 +1404,48 @@
   </si>
   <si>
     <t>BokTopic</t>
+  </si>
+  <si>
+    <t>Concept ID</t>
+  </si>
+  <si>
+    <t>Concept Name</t>
+  </si>
+  <si>
+    <t>Related Concepts</t>
+  </si>
+  <si>
+    <t>Dependent Variable;</t>
+  </si>
+  <si>
+    <t>Group;</t>
+  </si>
+  <si>
+    <t>Target Document;</t>
+  </si>
+  <si>
+    <t>Synonyms</t>
+  </si>
+  <si>
+    <t>Definitions</t>
+  </si>
+  <si>
+    <t>CON_0001</t>
+  </si>
+  <si>
+    <t>CON_0002</t>
+  </si>
+  <si>
+    <t>CON_0003</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Example Usages</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1519,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1566,7 +1611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1597,6 +1642,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1627,6 +1673,7 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1929,90 +1976,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="51.5" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
-        <v>134</v>
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>423</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>429</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
-        <v>135</v>
+        <v>435</v>
+      </c>
+      <c r="E1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="10" t="s">
+        <v>430</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="9" t="s">
-        <v>299</v>
+      <c r="F2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10" t="s">
+        <v>431</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C3" t="s">
         <v>300</v>
       </c>
-      <c r="D3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="9" t="s">
-        <v>302</v>
+      <c r="F3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="10" t="s">
+        <v>432</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>293</v>
+      <c r="F4" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Experiment!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -2021,6 +2064,290 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:G1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -2342,7 +2669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2437,7 +2764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2612,7 +2939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2748,12 +3075,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2831,7 +3158,7 @@
         <v>410</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2863,7 +3190,7 @@
         <v>410</v>
       </c>
       <c r="J3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2895,7 +3222,7 @@
         <v>410</v>
       </c>
       <c r="J4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3119,7 +3446,7 @@
         <v>410</v>
       </c>
       <c r="J11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3151,7 +3478,7 @@
         <v>410</v>
       </c>
       <c r="J12" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3183,7 +3510,7 @@
         <v>410</v>
       </c>
       <c r="J13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3215,7 +3542,7 @@
         <v>410</v>
       </c>
       <c r="J14" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3247,7 +3574,7 @@
         <v>410</v>
       </c>
       <c r="J15" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3279,7 +3606,7 @@
         <v>410</v>
       </c>
       <c r="J16" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3311,7 +3638,7 @@
         <v>410</v>
       </c>
       <c r="J17" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1">
@@ -3343,7 +3670,7 @@
         <v>410</v>
       </c>
       <c r="J18" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3375,7 +3702,7 @@
         <v>410</v>
       </c>
       <c r="J19" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3407,7 +3734,7 @@
         <v>410</v>
       </c>
       <c r="J20" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3439,7 +3766,7 @@
         <v>410</v>
       </c>
       <c r="J21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3471,7 +3798,7 @@
         <v>410</v>
       </c>
       <c r="J22" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1">
@@ -3503,7 +3830,7 @@
         <v>410</v>
       </c>
       <c r="J23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3535,7 +3862,7 @@
         <v>410</v>
       </c>
       <c r="J24" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3567,7 +3894,7 @@
         <v>403</v>
       </c>
       <c r="J25" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="10" customFormat="1">
@@ -3599,7 +3926,7 @@
         <v>410</v>
       </c>
       <c r="J26" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -3631,7 +3958,7 @@
         <v>410</v>
       </c>
       <c r="J27" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3663,7 +3990,7 @@
         <v>410</v>
       </c>
       <c r="J28" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="10" customFormat="1">
@@ -3695,7 +4022,7 @@
         <v>410</v>
       </c>
       <c r="J29" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3727,7 +4054,7 @@
         <v>410</v>
       </c>
       <c r="J30" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3759,7 +4086,7 @@
         <v>410</v>
       </c>
       <c r="J31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -3791,7 +4118,7 @@
         <v>410</v>
       </c>
       <c r="J32" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3823,7 +4150,7 @@
         <v>410</v>
       </c>
       <c r="J33" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3855,7 +4182,7 @@
         <v>410</v>
       </c>
       <c r="J34" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3887,7 +4214,7 @@
         <v>404</v>
       </c>
       <c r="J35" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3919,7 +4246,7 @@
         <v>410</v>
       </c>
       <c r="J36" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3951,7 +4278,7 @@
         <v>410</v>
       </c>
       <c r="J37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3983,7 +4310,7 @@
         <v>410</v>
       </c>
       <c r="J38" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4015,7 +4342,7 @@
         <v>405</v>
       </c>
       <c r="J39" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4047,7 +4374,7 @@
         <v>410</v>
       </c>
       <c r="J40" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -4079,7 +4406,7 @@
         <v>410</v>
       </c>
       <c r="J41" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -4111,7 +4438,7 @@
         <v>410</v>
       </c>
       <c r="J42" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="10" customFormat="1">
@@ -4143,7 +4470,7 @@
         <v>410</v>
       </c>
       <c r="J43" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -4175,7 +4502,7 @@
         <v>410</v>
       </c>
       <c r="J44" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -4207,7 +4534,7 @@
         <v>410</v>
       </c>
       <c r="J45" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -4239,7 +4566,7 @@
         <v>410</v>
       </c>
       <c r="J46" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -4271,7 +4598,7 @@
         <v>410</v>
       </c>
       <c r="J47" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -4303,7 +4630,7 @@
         <v>410</v>
       </c>
       <c r="J48" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -4335,7 +4662,7 @@
         <v>410</v>
       </c>
       <c r="J49" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="10" customFormat="1">
@@ -4367,7 +4694,7 @@
         <v>410</v>
       </c>
       <c r="J50" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -4399,7 +4726,7 @@
         <v>410</v>
       </c>
       <c r="J51" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -4431,7 +4758,7 @@
         <v>410</v>
       </c>
       <c r="J52" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -4463,7 +4790,7 @@
         <v>410</v>
       </c>
       <c r="J53" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -4495,7 +4822,7 @@
         <v>406</v>
       </c>
       <c r="J54" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -4527,7 +4854,7 @@
         <v>410</v>
       </c>
       <c r="J55" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -4559,7 +4886,7 @@
         <v>410</v>
       </c>
       <c r="J56" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="10" customFormat="1">
@@ -4591,7 +4918,7 @@
         <v>410</v>
       </c>
       <c r="J57" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -4623,7 +4950,7 @@
         <v>410</v>
       </c>
       <c r="J58" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -4655,7 +4982,7 @@
         <v>410</v>
       </c>
       <c r="J59" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -4687,7 +5014,7 @@
         <v>410</v>
       </c>
       <c r="J60" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -4719,7 +5046,7 @@
         <v>410</v>
       </c>
       <c r="J61" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -4751,7 +5078,7 @@
         <v>397</v>
       </c>
       <c r="J62" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -4783,7 +5110,7 @@
         <v>399</v>
       </c>
       <c r="J63" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="10" customFormat="1">
@@ -4815,7 +5142,7 @@
         <v>400</v>
       </c>
       <c r="J64" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4847,7 +5174,7 @@
         <v>401</v>
       </c>
       <c r="J65" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -4879,7 +5206,7 @@
         <v>402</v>
       </c>
       <c r="J66" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -4911,7 +5238,7 @@
         <v>410</v>
       </c>
       <c r="J67" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -4943,7 +5270,7 @@
         <v>410</v>
       </c>
       <c r="J68" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4975,7 +5302,7 @@
         <v>410</v>
       </c>
       <c r="J69" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -5007,7 +5334,7 @@
         <v>410</v>
       </c>
       <c r="J70" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="10" customFormat="1">
@@ -5039,7 +5366,7 @@
         <v>410</v>
       </c>
       <c r="J71" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -5071,7 +5398,7 @@
         <v>410</v>
       </c>
       <c r="J72" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -5103,7 +5430,7 @@
         <v>410</v>
       </c>
       <c r="J73" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -5135,7 +5462,7 @@
         <v>407</v>
       </c>
       <c r="J74" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="10" customFormat="1">
@@ -5167,7 +5494,7 @@
         <v>410</v>
       </c>
       <c r="J75" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -5199,7 +5526,7 @@
         <v>410</v>
       </c>
       <c r="J76" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -5231,7 +5558,7 @@
         <v>410</v>
       </c>
       <c r="J77" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -5263,7 +5590,7 @@
         <v>410</v>
       </c>
       <c r="J78" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -5295,7 +5622,7 @@
         <v>410</v>
       </c>
       <c r="J79" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="10" customFormat="1">
@@ -5327,7 +5654,7 @@
         <v>410</v>
       </c>
       <c r="J80" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -5359,7 +5686,7 @@
         <v>410</v>
       </c>
       <c r="J81" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -5391,7 +5718,7 @@
         <v>410</v>
       </c>
       <c r="J82" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -5423,7 +5750,7 @@
         <v>410</v>
       </c>
       <c r="J83" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -5496,10 +5823,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Experiment!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5681,12 +6101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5924,7 +6344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -6005,7 +6425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -6174,12 +6594,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6398,7 +6818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -6628,7 +7048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -7278,288 +7698,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="B9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>267</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="B10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>276</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11" t="s">
-        <v>245</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>278</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="B1:G1"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>